<commit_message>
Added UI and database
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyesh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyesh\Data-Analysis-Tool-Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF62A6D-0BEB-45B5-81A6-263AE495F7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69E6605-83F8-4112-BFCF-5F7C4A91A1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="1404" windowWidth="9948" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Project Title</t>
-  </si>
-  <si>
     <t>Data Analysis Tool Development</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>Software Version Control</t>
+  </si>
+  <si>
+    <t>Data Analysis Tool Development for Victoria State Accident Dataset</t>
   </si>
 </sst>
 </file>
@@ -568,28 +568,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -994,8 +994,8 @@
   </sheetPr>
   <dimension ref="B1:AP15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="73" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScale="81" zoomScaleNormal="89" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1016,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="2:42" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1039,37 +1039,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="32" t="s">
         <v>11</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="T2" s="34"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="34" t="s">
+      <c r="V2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="31"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
         <v>4</v>
@@ -1098,7 +1098,7 @@
       <c r="F3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="6" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="7" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7">
         <v>2</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7">
         <v>4</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="11" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
         <v>4</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="12" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="7">
         <v>8</v>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="13" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="7">
         <v>9</v>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7">
         <v>9</v>
@@ -1341,13 +1341,13 @@
     </row>
     <row r="15" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="9">
         <v>4</v>
       </c>
       <c r="D15" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>

</xml_diff>